<commit_message>
board renovations complete attempting to diagnose I2C again
</commit_message>
<xml_diff>
--- a/code/Small_scale/Pinout Translation.xlsx
+++ b/code/Small_scale/Pinout Translation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Pic 32 Pin #</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Card Detect 2</t>
+  </si>
+  <si>
+    <t>GPS Power (added wire)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +763,9 @@
       </c>
       <c r="B19" t="s">
         <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added port of data logging to small scale note: sequence of commits is not the same order as board was brought up due to some errors
</commit_message>
<xml_diff>
--- a/code/Small_scale/Pinout Translation.xlsx
+++ b/code/Small_scale/Pinout Translation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Pic 32 Pin #</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>GPS Power (added wire)</t>
+  </si>
+  <si>
+    <t>RA14</t>
+  </si>
+  <si>
+    <t>SD CS</t>
+  </si>
+  <si>
+    <t>RB14</t>
+  </si>
+  <si>
+    <t>CS</t>
   </si>
 </sst>
 </file>
@@ -251,8 +263,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0">
-  <autoFilter ref="A1:C32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C34" totalsRowShown="0">
+  <autoFilter ref="A1:C34"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Pic 32 Pin #"/>
     <tableColumn id="2" name="PIC32 Pin Description"/>
@@ -549,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,221 +697,243 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>50</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started changeover from blocking polled SD card writes to data portion interrupt driven and non-blocking polling code
</commit_message>
<xml_diff>
--- a/code/Small_scale/Pinout Translation.xlsx
+++ b/code/Small_scale/Pinout Translation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Pic 32 Pin #</t>
   </si>
@@ -99,15 +99,9 @@
     <t>RA0</t>
   </si>
   <si>
-    <t>PGED (reversed)</t>
-  </si>
-  <si>
     <t>RA1</t>
   </si>
   <si>
-    <t>PREC (reversed)</t>
-  </si>
-  <si>
     <t>RA2</t>
   </si>
   <si>
@@ -211,6 +205,9 @@
   </si>
   <si>
     <t>CS</t>
+  </si>
+  <si>
+    <t>SD Power Enable</t>
   </si>
 </sst>
 </file>
@@ -564,7 +561,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -700,10 +697,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -735,19 +732,16 @@
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,10 +749,10 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,10 +760,10 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,7 +771,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,10 +779,10 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,10 +790,10 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,7 +801,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,10 +809,10 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,10 +820,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,10 +831,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,10 +842,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,10 +853,10 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +864,7 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -878,10 +872,10 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,10 +883,10 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -908,10 +902,10 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -919,10 +913,10 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -930,10 +924,10 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>